<commit_message>
final freq and stress sweeps code and figures
</commit_message>
<xml_diff>
--- a/data/031024/10pct_0WSt_iCar/10pct_0WSt_iCar-StressSweep.xlsx
+++ b/data/031024/10pct_0WSt_iCar/10pct_0WSt_iCar-StressSweep.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petrus.kirsten\PycharmProjects\RheometerPlots\data\031024\10pct_0WSt_iCar\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DEFFEF-27CE-4BE8-8463-11D9649CD393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table p. 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Table p. 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true" refMode="A1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>t in s</t>
   </si>
   <si>
@@ -124,30 +128,30 @@
   </si>
   <si>
     <t>1-25</t>
+  </si>
+  <si>
+    <t>Seg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.00;-#,##0.00"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Segoe UI"/>
-      <b/>
-      <color rgb="FF000000"/>
-      <sz val="9"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Segoe UI"/>
-      <color rgb="FF000000"/>
-      <sz val="9"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,28 +171,32 @@
       <diagonal/>
     </border>
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -196,295 +204,615 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true"/>
+    <xf numFmtId="39" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>3990975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="685800" y="904875"/>
-          <a:ext cx="1219370" cy="1219370"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView zoomScale="100" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.44921875" customWidth="true"/>
-    <col min="2" max="2" width="7.44921875" customWidth="true"/>
-    <col min="3" max="3" width="7.44921875" customWidth="true"/>
-    <col min="4" max="4" width="7.44921875" customWidth="true"/>
-    <col min="5" max="5" width="7.44921875" customWidth="true"/>
-    <col min="6" max="6" width="7.44921875" customWidth="true"/>
-    <col min="7" max="7" width="7.44921875" customWidth="true"/>
-    <col min="8" max="8" width="7.44921875" customWidth="true"/>
-    <col min="9" max="9" width="7.44921875" customWidth="true"/>
-    <col min="10" max="10" width="7.44921875" customWidth="true"/>
-    <col min="11" max="11" width="7.44921875" customWidth="true"/>
-    <col min="12" max="12" width="7.44921875" customWidth="true"/>
-    <col min="13" max="13" width="1.4765625" customWidth="true"/>
+    <col min="1" max="1" width="3.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="374" customHeight="true"/>
-    <row r="2" ht="17.714" customHeight="true">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" ht="17.714" customHeight="true">
+      <c r="B2" s="4">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="C2" s="4">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4">
+        <v>870</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
+        <v>6.28</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="K2" s="4">
+        <v>8.1899999999999996E-4</v>
+      </c>
+      <c r="L2" s="4">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="4">
-        <v>77.599999999999994</v>
+        <v>93.6</v>
       </c>
       <c r="C3" s="4">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D3" s="4">
-        <v>870</v>
+        <v>928</v>
       </c>
       <c r="E3" s="4">
-        <v>200</v>
+        <v>121</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
       <c r="G3" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H3" s="4">
-        <v>0.23000000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="I3" s="4">
-        <v>0.12</v>
+        <v>0.17</v>
       </c>
       <c r="J3" s="4">
-        <v>0.012999999999999999</v>
+        <v>1.8599999999999998E-2</v>
       </c>
       <c r="K3" s="4">
-        <v>0.00081899999999999996</v>
+        <v>1.17E-3</v>
       </c>
       <c r="L3" s="4">
-        <v>1.3400000000000001</v>
-      </c>
-    </row>
-    <row r="4" ht="17.714" customHeight="true">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="4">
-        <v>93.599999999999994</v>
+        <v>110</v>
       </c>
       <c r="C4" s="4">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D4" s="4">
-        <v>928</v>
+        <v>951</v>
       </c>
       <c r="E4" s="4">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
       </c>
       <c r="G4" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H4" s="4">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="I4" s="4">
-        <v>0.17000000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="J4" s="4">
-        <v>0.018599999999999998</v>
+        <v>2.6499999999999999E-2</v>
       </c>
       <c r="K4" s="4">
-        <v>0.00117</v>
+        <v>1.67E-3</v>
       </c>
       <c r="L4" s="4">
-        <v>1.1799999999999999</v>
-      </c>
-    </row>
-    <row r="5" ht="17.714" customHeight="true">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="4">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="C5" s="4">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D5" s="4">
-        <v>951</v>
+        <v>968</v>
       </c>
       <c r="E5" s="4">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
       </c>
       <c r="G5" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H5" s="4">
         <v>0.12</v>
       </c>
       <c r="I5" s="4">
-        <v>0.25</v>
+        <v>0.37</v>
       </c>
       <c r="J5" s="4">
-        <v>0.026499999999999999</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="K5" s="4">
-        <v>0.00167</v>
+        <v>2.3900000000000002E-3</v>
       </c>
       <c r="L5" s="4">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="6" ht="17.714" customHeight="true">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="4">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="C6" s="4">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="D6" s="4">
-        <v>968</v>
+        <v>978</v>
       </c>
       <c r="E6" s="4">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
       </c>
       <c r="G6" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H6" s="4">
         <v>0.12</v>
       </c>
       <c r="I6" s="4">
-        <v>0.37</v>
+        <v>0.54</v>
       </c>
       <c r="J6" s="4">
-        <v>0.037999999999999999</v>
+        <v>5.4800000000000001E-2</v>
       </c>
       <c r="K6" s="4">
-        <v>0.0023900000000000002</v>
+        <v>3.4399999999999999E-3</v>
       </c>
       <c r="L6" s="4">
-        <v>0.91000000000000003</v>
-      </c>
-    </row>
-    <row r="7" ht="17.714" customHeight="true">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="4">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="C7" s="4">
-        <v>80</v>
+        <v>95.9</v>
       </c>
       <c r="D7" s="4">
-        <v>978</v>
+        <v>987</v>
       </c>
       <c r="E7" s="4">
         <v>116</v>
@@ -493,150 +821,150 @@
         <v>1</v>
       </c>
       <c r="G7" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H7" s="4">
         <v>0.12</v>
       </c>
       <c r="I7" s="4">
-        <v>0.54000000000000004</v>
+        <v>0.78</v>
       </c>
       <c r="J7" s="4">
-        <v>0.054800000000000001</v>
+        <v>7.9100000000000004E-2</v>
       </c>
       <c r="K7" s="4">
-        <v>0.0034399999999999999</v>
+        <v>4.9699999999999996E-3</v>
       </c>
       <c r="L7" s="4">
-        <v>0.80000000000000004</v>
-      </c>
-    </row>
-    <row r="8" ht="17.714" customHeight="true">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="4">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="C8" s="4">
-        <v>95.900000000000006</v>
+        <v>112</v>
       </c>
       <c r="D8" s="4">
-        <v>987</v>
+        <v>995</v>
       </c>
       <c r="E8" s="4">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
       </c>
       <c r="G8" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H8" s="4">
         <v>0.12</v>
       </c>
       <c r="I8" s="4">
-        <v>0.78000000000000003</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="J8" s="4">
-        <v>0.079100000000000004</v>
+        <v>0.11</v>
       </c>
       <c r="K8" s="4">
-        <v>0.0049699999999999996</v>
+        <v>7.1900000000000002E-3</v>
       </c>
       <c r="L8" s="4">
-        <v>0.70999999999999996</v>
-      </c>
-    </row>
-    <row r="9" ht="17.714" customHeight="true">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="4">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="C9" s="4">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="D9" s="4">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E9" s="4">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
       <c r="G9" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H9" s="4">
         <v>0.12</v>
       </c>
       <c r="I9" s="4">
-        <v>1.1399999999999999</v>
+        <v>1.66</v>
       </c>
       <c r="J9" s="4">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
       <c r="K9" s="4">
-        <v>0.0071900000000000002</v>
+        <v>1.04E-2</v>
       </c>
       <c r="L9" s="4">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="10" ht="17.714" customHeight="true">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="4">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="C10" s="4">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="D10" s="4">
-        <v>1000</v>
+        <v>1010</v>
       </c>
       <c r="E10" s="4">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
       </c>
       <c r="G10" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H10" s="4">
         <v>0.12</v>
       </c>
       <c r="I10" s="4">
-        <v>1.6599999999999999</v>
+        <v>2.42</v>
       </c>
       <c r="J10" s="4">
-        <v>0.17000000000000001</v>
+        <v>0.24</v>
       </c>
       <c r="K10" s="4">
-        <v>0.0104</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="L10" s="4">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="11" ht="17.714" customHeight="true">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="4">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="C11" s="4">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="D11" s="4">
-        <v>1010</v>
+        <v>1020</v>
       </c>
       <c r="E11" s="4">
         <v>117</v>
@@ -645,109 +973,109 @@
         <v>1</v>
       </c>
       <c r="G11" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H11" s="4">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="I11" s="4">
-        <v>2.4199999999999999</v>
+        <v>3.52</v>
       </c>
       <c r="J11" s="4">
-        <v>0.23999999999999999</v>
+        <v>0.35</v>
       </c>
       <c r="K11" s="4">
-        <v>0.014999999999999999</v>
+        <v>2.1700000000000001E-2</v>
       </c>
       <c r="L11" s="4">
-        <v>0.52000000000000002</v>
-      </c>
-    </row>
-    <row r="12" ht="17.714" customHeight="true">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="4">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="C12" s="4">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="D12" s="4">
-        <v>1020</v>
+        <v>1030</v>
       </c>
       <c r="E12" s="4">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
       </c>
       <c r="G12" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H12" s="4">
         <v>0.11</v>
       </c>
       <c r="I12" s="4">
-        <v>3.52</v>
+        <v>5.13</v>
       </c>
       <c r="J12" s="4">
-        <v>0.34999999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="K12" s="4">
-        <v>0.021700000000000001</v>
+        <v>3.1399999999999997E-2</v>
       </c>
       <c r="L12" s="4">
-        <v>0.46999999999999997</v>
-      </c>
-    </row>
-    <row r="13" ht="17.714" customHeight="true">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="4">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="C13" s="4">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="D13" s="4">
         <v>1030</v>
       </c>
       <c r="E13" s="4">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
       </c>
       <c r="G13" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H13" s="4">
         <v>0.11</v>
       </c>
       <c r="I13" s="4">
-        <v>5.1299999999999999</v>
+        <v>7.48</v>
       </c>
       <c r="J13" s="4">
-        <v>0.5</v>
+        <v>0.73</v>
       </c>
       <c r="K13" s="4">
-        <v>0.031399999999999997</v>
+        <v>4.5600000000000002E-2</v>
       </c>
       <c r="L13" s="4">
-        <v>0.42999999999999999</v>
-      </c>
-    </row>
-    <row r="14" ht="17.714" customHeight="true">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="4">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="C14" s="4">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="D14" s="4">
         <v>1030</v>
@@ -759,528 +1087,485 @@
         <v>1</v>
       </c>
       <c r="G14" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H14" s="4">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="I14" s="4">
-        <v>7.4800000000000004</v>
+        <v>10.9</v>
       </c>
       <c r="J14" s="4">
-        <v>0.72999999999999998</v>
+        <v>1.06</v>
       </c>
       <c r="K14" s="4">
-        <v>0.045600000000000002</v>
+        <v>6.6699999999999995E-2</v>
       </c>
       <c r="L14" s="4">
-        <v>0.39000000000000001</v>
-      </c>
-    </row>
-    <row r="15" ht="17.714" customHeight="true">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="4">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="C15" s="4">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="D15" s="4">
         <v>1030</v>
       </c>
       <c r="E15" s="4">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>
       </c>
       <c r="G15" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H15" s="4">
         <v>0.12</v>
       </c>
       <c r="I15" s="4">
-        <v>10.9</v>
+        <v>15.9</v>
       </c>
       <c r="J15" s="4">
-        <v>1.0600000000000001</v>
+        <v>1.55</v>
       </c>
       <c r="K15" s="4">
-        <v>0.066699999999999995</v>
+        <v>9.7199999999999995E-2</v>
       </c>
       <c r="L15" s="4">
-        <v>0.34999999999999998</v>
-      </c>
-    </row>
-    <row r="16" ht="17.714" customHeight="true">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="4">
-        <v>285</v>
+        <v>301</v>
       </c>
       <c r="C16" s="4">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="D16" s="4">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="E16" s="4">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
       </c>
       <c r="G16" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H16" s="4">
         <v>0.12</v>
       </c>
       <c r="I16" s="4">
-        <v>15.9</v>
+        <v>23.1</v>
       </c>
       <c r="J16" s="4">
-        <v>1.55</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="K16" s="4">
-        <v>0.097199999999999995</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="L16" s="4">
-        <v>0.33000000000000002</v>
-      </c>
-    </row>
-    <row r="17" ht="17.714" customHeight="true">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="4">
-        <v>301</v>
+        <v>317</v>
       </c>
       <c r="C17" s="4">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="D17" s="4">
-        <v>1020</v>
+        <v>1010</v>
       </c>
       <c r="E17" s="4">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="F17" s="4">
         <v>1</v>
       </c>
       <c r="G17" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H17" s="4">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="I17" s="4">
-        <v>23.100000000000001</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="J17" s="4">
-        <v>2.2599999999999998</v>
+        <v>3.34</v>
       </c>
       <c r="K17" s="4">
-        <v>0.14000000000000001</v>
+        <v>0.21</v>
       </c>
       <c r="L17" s="4">
-        <v>0.29999999999999999</v>
-      </c>
-    </row>
-    <row r="18" ht="17.714" customHeight="true">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="4">
-        <v>317</v>
+        <v>333</v>
       </c>
       <c r="C18" s="4">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="D18" s="4">
-        <v>1010</v>
+        <v>992</v>
       </c>
       <c r="E18" s="4">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
       </c>
       <c r="G18" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H18" s="4">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="I18" s="4">
-        <v>33.700000000000003</v>
+        <v>49.2</v>
       </c>
       <c r="J18" s="4">
-        <v>3.3399999999999999</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="K18" s="4">
-        <v>0.20999999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="L18" s="4">
-        <v>0.27000000000000002</v>
-      </c>
-    </row>
-    <row r="19" ht="17.714" customHeight="true">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="4">
-        <v>333</v>
+        <v>349</v>
       </c>
       <c r="C19" s="4">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="D19" s="4">
-        <v>992</v>
+        <v>961</v>
       </c>
       <c r="E19" s="4">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
       </c>
       <c r="G19" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H19" s="4">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="I19" s="4">
-        <v>49.200000000000003</v>
+        <v>71.599999999999994</v>
       </c>
       <c r="J19" s="4">
-        <v>4.9400000000000004</v>
+        <v>7.42</v>
       </c>
       <c r="K19" s="4">
-        <v>0.31</v>
+        <v>0.47</v>
       </c>
       <c r="L19" s="4">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="20" ht="17.714" customHeight="true">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="4">
-        <v>349</v>
+        <v>365</v>
       </c>
       <c r="C20" s="4">
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="D20" s="4">
-        <v>961</v>
+        <v>905</v>
       </c>
       <c r="E20" s="4">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
       </c>
       <c r="G20" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H20" s="4">
-        <v>0.14999999999999999</v>
+        <v>0.18</v>
       </c>
       <c r="I20" s="4">
-        <v>71.599999999999994</v>
+        <v>104</v>
       </c>
       <c r="J20" s="4">
-        <v>7.4199999999999999</v>
+        <v>11.4</v>
       </c>
       <c r="K20" s="4">
-        <v>0.46999999999999997</v>
+        <v>0.72</v>
       </c>
       <c r="L20" s="4">
-        <v>0.23000000000000001</v>
-      </c>
-    </row>
-    <row r="21" ht="17.714" customHeight="true">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="4">
-        <v>365</v>
+        <v>381</v>
       </c>
       <c r="C21" s="4">
-        <v>304</v>
+        <v>320</v>
       </c>
       <c r="D21" s="4">
-        <v>905</v>
+        <v>813</v>
       </c>
       <c r="E21" s="4">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
       </c>
       <c r="G21" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H21" s="4">
-        <v>0.17999999999999999</v>
+        <v>0.22</v>
       </c>
       <c r="I21" s="4">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="J21" s="4">
-        <v>11.4</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="K21" s="4">
-        <v>0.71999999999999997</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="L21" s="4">
-        <v>0.23000000000000001</v>
-      </c>
-    </row>
-    <row r="22" ht="17.714" customHeight="true">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="4">
-        <v>381</v>
+        <v>397</v>
       </c>
       <c r="C22" s="4">
-        <v>320</v>
+        <v>336</v>
       </c>
       <c r="D22" s="4">
-        <v>813</v>
+        <v>654</v>
       </c>
       <c r="E22" s="4">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
       </c>
       <c r="G22" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H22" s="4">
-        <v>0.22</v>
+        <v>0.31</v>
       </c>
       <c r="I22" s="4">
-        <v>152</v>
+        <v>222</v>
       </c>
       <c r="J22" s="4">
-        <v>18.399999999999999</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="K22" s="4">
-        <v>1.1599999999999999</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="L22" s="4">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="23" ht="17.714" customHeight="true">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="4">
-        <v>397</v>
+        <v>413</v>
       </c>
       <c r="C23" s="4">
-        <v>336</v>
+        <v>352</v>
       </c>
       <c r="D23" s="4">
-        <v>654</v>
+        <v>344</v>
       </c>
       <c r="E23" s="4">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
       </c>
       <c r="G23" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H23" s="4">
-        <v>0.31</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I23" s="4">
-        <v>222</v>
+        <v>323</v>
       </c>
       <c r="J23" s="4">
-        <v>32.700000000000003</v>
+        <v>82.6</v>
       </c>
       <c r="K23" s="4">
-        <v>2.0499999999999998</v>
+        <v>5.19</v>
       </c>
       <c r="L23" s="4">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="24" ht="17.714" customHeight="true">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B24" s="4">
-        <v>413</v>
+        <v>429</v>
       </c>
       <c r="C24" s="4">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="D24" s="4">
-        <v>344</v>
+        <v>6.19</v>
       </c>
       <c r="E24" s="4">
-        <v>200</v>
+        <v>63</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
       </c>
       <c r="G24" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H24" s="4">
-        <v>0.57999999999999996</v>
+        <v>10.6</v>
       </c>
       <c r="I24" s="4">
-        <v>323</v>
+        <v>471</v>
       </c>
       <c r="J24" s="4">
-        <v>82.599999999999994</v>
+        <v>742</v>
       </c>
       <c r="K24" s="4">
-        <v>5.1900000000000004</v>
+        <v>46.6</v>
       </c>
       <c r="L24" s="4">
-        <v>0.35999999999999999</v>
-      </c>
-    </row>
-    <row r="25" ht="17.714" customHeight="true">
+        <v>9.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="4">
-        <v>429</v>
+        <v>445</v>
       </c>
       <c r="C25" s="4">
-        <v>368</v>
+        <v>384</v>
       </c>
       <c r="D25" s="4">
-        <v>6.1900000000000004</v>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="E25" s="4">
-        <v>63</v>
+        <v>18.8</v>
       </c>
       <c r="F25" s="4">
         <v>1</v>
       </c>
       <c r="G25" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H25" s="4">
-        <v>10.6</v>
+        <v>1000</v>
       </c>
       <c r="I25" s="4">
-        <v>471</v>
+        <v>686</v>
       </c>
       <c r="J25" s="4">
-        <v>742</v>
+        <v>3200</v>
       </c>
       <c r="K25" s="4">
-        <v>46.600000000000001</v>
+        <v>201</v>
       </c>
       <c r="L25" s="4">
-        <v>0.092499999999999999</v>
-      </c>
-    </row>
-    <row r="26" ht="17.714" customHeight="true">
+        <v>2.8799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="4">
-        <v>445</v>
+        <v>461</v>
       </c>
       <c r="C26" s="4">
-        <v>384</v>
+        <v>400</v>
       </c>
       <c r="D26" s="4">
-        <v>0.018800000000000001</v>
+        <v>8.9300000000000004E-3</v>
       </c>
       <c r="E26" s="4">
-        <v>18.800000000000001</v>
+        <v>8.93</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
       </c>
       <c r="G26" s="4">
-        <v>6.2800000000000002</v>
+        <v>6.28</v>
       </c>
       <c r="H26" s="4">
         <v>1000</v>
       </c>
       <c r="I26" s="4">
-        <v>686</v>
+        <v>1000</v>
       </c>
       <c r="J26" s="4">
-        <v>3200</v>
+        <v>8140</v>
       </c>
       <c r="K26" s="4">
-        <v>201</v>
+        <v>511</v>
       </c>
       <c r="L26" s="4">
-        <v>0.028799999999999999</v>
-      </c>
-    </row>
-    <row r="27" ht="17.714" customHeight="true">
-      <c r="A27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="4">
-        <v>461</v>
-      </c>
-      <c r="C27" s="4">
-        <v>400</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0.0089300000000000004</v>
-      </c>
-      <c r="E27" s="4">
-        <v>8.9299999999999997</v>
-      </c>
-      <c r="F27" s="4">
-        <v>1</v>
-      </c>
-      <c r="G27" s="4">
-        <v>6.2800000000000002</v>
-      </c>
-      <c r="H27" s="4">
-        <v>1000</v>
-      </c>
-      <c r="I27" s="4">
-        <v>1000</v>
-      </c>
-      <c r="J27" s="4">
-        <v>8140</v>
-      </c>
-      <c r="K27" s="4">
-        <v>511</v>
-      </c>
-      <c r="L27" s="4">
-        <v>0.0567</v>
+        <v>5.67E-2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.0" right="0.0" top="0.0" bottom="0.0" header="0.0" footer="0.0"/>
-  <pageSetup paperSize="9" scale="87" orientation="portrait"/>
-  <headerFooter>
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="87" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="27" max="16383" man="true"/>
+    <brk id="26" max="16383" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>